<commit_message>
Added till 20/04/2021[Week 3 completed]
</commit_message>
<xml_diff>
--- a/Week 3/Week 3  Plan.xlsx
+++ b/Week 3/Week 3  Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Week 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E602284-C24B-434C-9290-A30AC7F60A06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6766F067-1554-4F2B-996D-B25A0AF33CB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>https://www.geeksforgeeks.org/nth-node-from-the-end-of-a-linked-list/</t>
   </si>
@@ -110,34 +110,13 @@
   </si>
   <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/sum-of-two-linked-lists/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/multiply-two-numbers-represented-linked-lists/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/a-linked-list-with-next-and-arbit-pointer/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/delete-n-nodes-after-m-nodes-of-a-linked-list/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/merge-a-linked-list-into-another-linked-list-at-alternate-positions/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/flattening-a-linked-list/</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/xor-linked-list-a-memory-efficient-doubly-linked-list-set-1/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -171,19 +150,6 @@
       <u/>
       <sz val="12"/>
       <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -229,11 +195,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,10 +231,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,10 +449,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -983,10 +946,12 @@
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="11"/>
+      <c r="A23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1003,10 +968,12 @@
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="11"/>
+      <c r="A24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1023,10 +990,12 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="11"/>
+      <c r="A25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1043,10 +1012,12 @@
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="11"/>
+      <c r="A26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1063,10 +1034,12 @@
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="11"/>
+      <c r="A27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -1083,10 +1056,12 @@
       <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="11"/>
+      <c r="A28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1103,152 +1078,125 @@
       <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="12"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="12"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="12"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="12"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1265,7 +1213,7 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1282,7 +1230,7 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -1299,7 +1247,7 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -1316,7 +1264,7 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -1333,7 +1281,7 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1350,7 +1298,7 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -1367,7 +1315,7 @@
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1384,7 +1332,7 @@
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -1401,7 +1349,7 @@
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -1418,7 +1366,7 @@
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -1435,7 +1383,7 @@
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1452,7 +1400,7 @@
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -1502,125 +1450,6 @@
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="12"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="12"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="12"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="12"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="6"/>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B57" s="12"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1644,22 +1473,15 @@
     <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A30" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A31" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A35" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="A17" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A23" r:id="rId28" xr:uid="{A1FC35BA-F671-4963-AB55-DA4842CE1DDD}"/>
-    <hyperlink ref="A24" r:id="rId29" xr:uid="{8BBF2C76-1B9F-4B17-A23A-4F68E7819936}"/>
-    <hyperlink ref="A25" r:id="rId30" xr:uid="{2A7793C7-3657-4A21-8F61-27AD2B05A7B2}"/>
-    <hyperlink ref="A28" r:id="rId31" xr:uid="{F29A000E-F4C3-4584-8626-5407F79F07D8}"/>
-    <hyperlink ref="A27" r:id="rId32" xr:uid="{0C2BBA35-D266-4974-83A8-E63421D1E07F}"/>
-    <hyperlink ref="A26" r:id="rId33" xr:uid="{B7744941-43D2-49CA-B4FC-60C1A1161A1C}"/>
-    <hyperlink ref="A29" r:id="rId34" xr:uid="{492C619D-6AC5-4E2B-94FC-34A015166DB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>